<commit_message>
Updated table summarizing transportation/manipulation approaches
</commit_message>
<xml_diff>
--- a/Literature Review/Summary of state of the art.xlsx
+++ b/Literature Review/Summary of state of the art.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4731D4-9A59-4BAE-B890-990E6430C886}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA3163A-2C19-4E24-97D1-55CB8068C964}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
   <si>
     <t>Paper ID</t>
   </si>
@@ -88,42 +88,21 @@
     <t>Distributed</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>PD nonlinear</t>
   </si>
   <si>
     <t>Admittance control</t>
   </si>
   <si>
-    <t>Admittance control + MPC</t>
-  </si>
-  <si>
     <t>PID</t>
   </si>
   <si>
     <t>PD (trajectory) + LQR (formation) + PD (agent pose)</t>
   </si>
   <si>
-    <t>Spring-damper Model or Potential field</t>
-  </si>
-  <si>
     <t>LQR (leader) +  LQR &amp; PD (follower)</t>
   </si>
   <si>
-    <t>MPC (velocity) + PI (propulsion) + penalty force &amp; VFH+- (collision)</t>
-  </si>
-  <si>
-    <t>Cascaded PID (formation) + potential field (collision)</t>
-  </si>
-  <si>
-    <t>PID + feedforward compensation + potential field (collision)</t>
-  </si>
-  <si>
-    <t>min. Snap &amp; min. Duration</t>
-  </si>
-  <si>
     <t>Distributed wrench controller</t>
   </si>
   <si>
@@ -134,6 +113,81 @@
   </si>
   <si>
     <t>MPC receding horizon</t>
+  </si>
+  <si>
+    <t>Calculation of workspace of valid trajectories, no info on how a trajectory is selected</t>
+  </si>
+  <si>
+    <t>PID + feedforward compensation + potential field (collision avoidance)</t>
+  </si>
+  <si>
+    <t>Cascaded PID (formation) + potential field (collision avoidance)</t>
+  </si>
+  <si>
+    <t>Analytical feedback control strategy, dynamic motion primitives (collision avoidance)</t>
+  </si>
+  <si>
+    <t>Force estimation + Admittance control + MPC</t>
+  </si>
+  <si>
+    <t>Agents' state</t>
+  </si>
+  <si>
+    <t>Agents' state, cable force</t>
+  </si>
+  <si>
+    <t>Agents' state, obstacle pose</t>
+  </si>
+  <si>
+    <t>Internal force</t>
+  </si>
+  <si>
+    <t>Control force = PD + bias force</t>
+  </si>
+  <si>
+    <t>Continual calculation of setpoint for group center position given desired payload pose and velocity</t>
+  </si>
+  <si>
+    <t>Agents' state, load state</t>
+  </si>
+  <si>
+    <t>Payload trajectory set at beginning</t>
+  </si>
+  <si>
+    <t>Payload trajectory set at beginning (piecewise polynomial over time)</t>
+  </si>
+  <si>
+    <t>Payload trajectory set at beginning (polynomial over time), modified by dynamic motion primitives</t>
+  </si>
+  <si>
+    <t>Spring-damper (PD) Model or Potential field</t>
+  </si>
+  <si>
+    <t>Payload path set at beginning, continual calculation of velocity</t>
+  </si>
+  <si>
+    <t>Agents' state with respect to formation, load pose, some communication with neighbors</t>
+  </si>
+  <si>
+    <t>MPC &amp; PI (velocity) + penalty force &amp; VFH+- (collision avoidance)</t>
+  </si>
+  <si>
+    <t>Waypoints pre-specified, calculate reference trajectory subject to min. Snap (QP) &amp; min. Duration (Coordinate descent)</t>
+  </si>
+  <si>
+    <t>Trajectory planning addressed in Lai, Wang, and Chen (2017) and Lai et al. (2016)</t>
+  </si>
+  <si>
+    <t>Body state (Agents' state)</t>
+  </si>
+  <si>
+    <t>Agents' state, load geometry (no force/torque measurements)</t>
+  </si>
+  <si>
+    <t>Continual calculation of trajectory by leader given a desired payload final pose.</t>
+  </si>
+  <si>
+    <t>Predefined trajectory tracking; Point-to-Point path planning</t>
   </si>
 </sst>
 </file>
@@ -463,9 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -473,7 +525,7 @@
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -521,13 +573,13 @@
         <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -547,13 +599,13 @@
         <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -573,13 +625,13 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -599,13 +651,13 @@
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -625,13 +677,13 @@
         <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -651,13 +703,13 @@
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -677,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -691,7 +743,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -703,13 +755,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -729,13 +781,13 @@
         <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -749,19 +801,19 @@
         <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -781,13 +833,13 @@
         <v>21</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -807,13 +859,13 @@
         <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -833,13 +885,13 @@
         <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -859,13 +911,13 @@
         <v>19</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -885,13 +937,13 @@
         <v>21</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -911,13 +963,13 @@
         <v>20</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completion of reflection on literature survey findings, initial qualitative work on problem formulation
</commit_message>
<xml_diff>
--- a/Literature Review/Summary of state of the art.xlsx
+++ b/Literature Review/Summary of state of the art.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA3163A-2C19-4E24-97D1-55CB8068C964}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260519F7-CEA0-472A-9DFE-1ED0BDA4B48A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,12 +211,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -231,10 +237,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,16 +526,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+    <col min="7" max="7" width="66.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -610,7 +621,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -619,264 +630,264 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="G9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>48</v>
+      <c r="F13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>17</v>
@@ -885,44 +896,44 @@
         <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
@@ -931,24 +942,24 @@
         <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
@@ -957,22 +968,25 @@
         <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
+    <sortCondition ref="E2:E17"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added bibliography entry for new paper by Klausen et al. (2018).
</commit_message>
<xml_diff>
--- a/Literature Review/Summary of state of the art.xlsx
+++ b/Literature Review/Summary of state of the art.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260519F7-CEA0-472A-9DFE-1ED0BDA4B48A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1E76C2-121A-46D2-8D1D-E371336C20F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>Paper ID</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>Predefined trajectory tracking; Point-to-Point path planning</t>
+  </si>
+  <si>
+    <t>Agent positions in formation and common velocity set at beginning</t>
+  </si>
+  <si>
+    <t>Passivity-based PD (internal feedback) +  feedback control (formation)</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,6 +989,32 @@
         <v>53</v>
       </c>
     </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
     <sortCondition ref="E2:E17"/>

</xml_diff>